<commit_message>
Ultima actualizacion cambios menores
</commit_message>
<xml_diff>
--- a/data/loggin.xlsx
+++ b/data/loggin.xlsx
@@ -1,38 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bconline-my.sharepoint.com/personal/cristian_echevarria_oneasg_com/Documents/Documents/Proyectos_Python/PysimpleGUI/Proyectos/mantto_feeder/data/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="11_A1694C168271E7E66D7017CAD8CBD5ADA9DCB3B3" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BA28A91E-DD88-40FE-8546-5A397EDB4A33}"/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="6000" yWindow="1395" windowWidth="21270" windowHeight="11055" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -48,67 +44,114 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>161925</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="2114550" cy="2162175"/>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Image 1" descr="Picture">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr/>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print"/>
+<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <oneCellAnchor>
+    <from>
+      <col>1</col>
+      <colOff>0</colOff>
+      <row>1</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="2114550" cy="2162175"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr descr="Picture" id="1" name="Image 1"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId1"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="771525" y="152400"/>
-          <a:ext cx="2114550" cy="2162175"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-</xdr:wsDr>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+</wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -395,19 +438,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1"/>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter>
-    <oddFooter>&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K0000FF This data is internal to Brunswick.</oddFooter>
-  </headerFooter>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>